<commit_message>
sample num 4 is cleaned up
</commit_message>
<xml_diff>
--- a/Test-Data/Example4.xlsx
+++ b/Test-Data/Example4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI-MRO\Data\Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32265346-7E05-4FF7-AA97-D8ED01E20195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E675A8-AE3B-40E2-B794-531379F1C6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="2400" yWindow="5690" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
@@ -838,20 +838,20 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="3"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -874,7 +874,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -899,7 +899,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>102</v>
@@ -925,7 +925,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>103</v>
@@ -940,8 +940,7 @@
         <v>45748</v>
       </c>
       <c r="E4" s="9">
-        <f>C4+0.81</f>
-        <v>1.1711111111111112</v>
+        <v>0.1711111111111111</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
@@ -951,7 +950,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -966,8 +965,7 @@
         <v>45748</v>
       </c>
       <c r="E5" s="9">
-        <f>C5+0.74</f>
-        <v>1.1393055555555556</v>
+        <v>0.13930555555555554</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
@@ -977,7 +975,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -992,18 +990,17 @@
         <v>45748</v>
       </c>
       <c r="E6" s="9">
-        <f>C6+0.391</f>
-        <v>0.86669444444444443</v>
+        <v>0.86668981481481477</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>0.39100000000000001</v>
+        <v>0.39099537037037035</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1028,7 +1025,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1053,7 +1050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1068,18 +1065,17 @@
         <v>45748</v>
       </c>
       <c r="E9" s="9">
-        <f>C9+0.6</f>
-        <v>1.1625000000000001</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.6</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1105,7 +1101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1120,18 +1116,17 @@
         <v>45749</v>
       </c>
       <c r="E11" s="9">
-        <f>C11+0.621</f>
-        <v>1.3154444444444444</v>
+        <v>0.31543981481481481</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>0.621</v>
+        <v>0.62099537037037034</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1146,18 +1141,17 @@
         <v>45749</v>
       </c>
       <c r="E12" s="9">
-        <f>C12+0.59</f>
-        <v>1.3191666666666666</v>
+        <v>0.31916666666666665</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.59000000000000008</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1172,18 +1166,17 @@
         <v>45749</v>
       </c>
       <c r="E13" s="9">
-        <f>C13+0.655</f>
-        <v>1.4327777777777779</v>
+        <v>0.43277777777777776</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>0.65500000000000014</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1198,18 +1191,17 @@
         <v>45749</v>
       </c>
       <c r="E14" s="9">
-        <f>C14+0.865</f>
-        <v>1.6740277777777779</v>
+        <v>0.67402777777777778</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>0.8650000000000001</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1224,18 +1216,17 @@
         <v>45749</v>
       </c>
       <c r="E15" s="9">
-        <f>C15+0.677</f>
-        <v>1.4790833333333335</v>
+        <v>0.47907407407407404</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="0"/>
-        <v>0.67700000000000016</v>
+        <v>0.67699074074074073</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1250,18 +1241,17 @@
         <v>45749</v>
       </c>
       <c r="E16" s="9">
-        <f>C16+0.788</f>
-        <v>1.6039722222222221</v>
+        <v>0.60396990740740741</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="0"/>
-        <v>0.78799999999999992</v>
+        <v>0.7879976851851852</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1276,18 +1266,17 @@
         <v>45749</v>
       </c>
       <c r="E17" s="9">
-        <f>C17+0.73</f>
-        <v>1.5876388888888888</v>
+        <v>0.58763888888888893</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>0.73</v>
+        <v>0.73000000000000009</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1302,8 +1291,7 @@
         <v>45749</v>
       </c>
       <c r="E18" s="9">
-        <f>C18+0.85</f>
-        <v>1.7354166666666666</v>
+        <v>0.73541666666666661</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
@@ -1313,7 +1301,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1338,7 +1326,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1363,7 +1351,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1388,131 +1376,131 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B53" s="8"/>
       <c r="D53" s="8"/>
     </row>
@@ -1529,18 +1517,18 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="3"/>
-    <col min="4" max="4" width="10.875" style="4"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1557,7 +1545,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1581,7 +1569,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1605,7 +1593,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1617,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1641,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1665,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1701,7 +1689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1725,7 +1713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1749,7 +1737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1773,7 +1761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1797,7 +1785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1821,7 +1809,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1833,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1869,7 +1857,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1893,7 +1881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1917,7 +1905,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1941,7 +1929,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +1953,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1989,7 +1977,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2039,7 +2027,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2064,7 +2052,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2077,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2114,7 +2102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -2156,13 +2144,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>109</v>
       </c>
@@ -2170,7 +2158,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2181,7 +2169,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2192,7 +2180,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2203,7 +2191,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2214,7 +2202,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2225,7 +2213,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2236,7 +2224,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2247,7 +2235,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2258,7 +2246,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2269,7 +2257,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2280,7 +2268,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2291,7 +2279,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2302,7 +2290,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2313,7 +2301,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2324,7 +2312,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2335,7 +2323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2346,7 +2334,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2357,7 +2345,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2368,7 +2356,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2379,7 +2367,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2390,7 +2378,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2401,7 +2389,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2412,7 +2400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2423,7 +2411,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2434,7 +2422,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2445,7 +2433,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2456,7 +2444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2467,7 +2455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2478,7 +2466,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2489,7 +2477,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2500,7 +2488,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2511,7 +2499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2522,7 +2510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2533,7 +2521,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2544,7 +2532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2555,7 +2543,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>

</xml_diff>